<commit_message>
Burndown charts added for week 3
</commit_message>
<xml_diff>
--- a/burndown_charts/StoryPoint Burndown.xlsx
+++ b/burndown_charts/StoryPoint Burndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nachiketbhagwat/Desktop/Burndown/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nachiketbhagwat/Study/Software_Enginnering/newgit/Software-Project/burndown_charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -223,18 +223,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$27:$I$27</c:f>
+              <c:f>Sheet1!$B$28:$I$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>186.0</c:v>
+                  <c:v>191.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>185.0</c:v>
+                  <c:v>191.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>141.0</c:v>
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -267,12 +270,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$28:$I$28</c:f>
+              <c:f>Sheet1!$B$29:$I$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>186.0</c:v>
+                  <c:v>191.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>159.43</c:v>
@@ -309,11 +312,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2109835632"/>
-        <c:axId val="2109838912"/>
+        <c:axId val="-2129485104"/>
+        <c:axId val="-2085087520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109835632"/>
+        <c:axId val="-2129485104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -354,7 +357,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109838912"/>
+        <c:crossAx val="-2085087520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -362,7 +365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109838912"/>
+        <c:axId val="-2085087520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,7 +415,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109835632"/>
+        <c:crossAx val="-2129485104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1051,7 +1054,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1337,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1392,6 +1395,9 @@
       <c r="D2">
         <v>8</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1406,6 +1412,9 @@
       <c r="D3">
         <v>5</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1420,6 +1429,9 @@
       <c r="D4">
         <v>3</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -1434,6 +1446,9 @@
       <c r="D5">
         <v>3</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -1448,6 +1463,9 @@
       <c r="D6">
         <v>13</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -1462,6 +1480,9 @@
       <c r="D7">
         <v>5</v>
       </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1476,6 +1497,9 @@
       <c r="D8">
         <v>8</v>
       </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1490,6 +1514,9 @@
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1504,6 +1531,9 @@
       <c r="D10">
         <v>0</v>
       </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1518,6 +1548,9 @@
       <c r="D11">
         <v>0</v>
       </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1532,6 +1565,9 @@
       <c r="D12">
         <v>0</v>
       </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1546,6 +1582,9 @@
       <c r="D13">
         <v>0</v>
       </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1560,6 +1599,9 @@
       <c r="D14">
         <v>0</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1574,6 +1616,9 @@
       <c r="D15">
         <v>0</v>
       </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1588,6 +1633,9 @@
       <c r="D16">
         <v>0</v>
       </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -1602,6 +1650,9 @@
       <c r="D17">
         <v>0</v>
       </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -1616,6 +1667,9 @@
       <c r="D18">
         <v>0</v>
       </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1630,6 +1684,9 @@
       <c r="D19">
         <v>0</v>
       </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -1644,6 +1701,9 @@
       <c r="D20">
         <v>0</v>
       </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -1658,6 +1718,9 @@
       <c r="D21">
         <v>0</v>
       </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -1672,6 +1735,9 @@
       <c r="D22">
         <v>0</v>
       </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -1686,6 +1752,9 @@
       <c r="D23">
         <v>0</v>
       </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -1700,6 +1769,9 @@
       <c r="D24">
         <v>0</v>
       </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -1714,6 +1786,9 @@
       <c r="D25">
         <v>0</v>
       </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -1728,42 +1803,65 @@
       <c r="D26">
         <v>0</v>
       </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
       <c r="B27">
-        <f>SUM(B2:B26)</f>
-        <v>186</v>
+        <v>5</v>
       </c>
       <c r="C27">
-        <v>185</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>141</v>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28">
-        <v>186</v>
+        <f>SUM(B2:B27)</f>
+        <v>191</v>
       </c>
       <c r="C28">
+        <v>191</v>
+      </c>
+      <c r="D28">
+        <v>146</v>
+      </c>
+      <c r="E28">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>191</v>
+      </c>
+      <c r="C29">
         <v>159.43</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>132.86000000000001</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>106.29</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>79.72</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>53.15</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <v>26.58</v>
       </c>
-      <c r="I28">
+      <c r="I29">
         <v>0</v>
       </c>
     </row>

</xml_diff>